<commit_message>
TestNG Framework class 04 commit 1
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/hrmsTestdata.xlsx
+++ b/src/test/resources/testdata/hrmsTestdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jama\Desktop\Bootcamps\Syntax\SyntaxMavenProject\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F71D0229-EAF4-4B3F-A82C-4BAAA498845B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D75D0FD8-4E58-4F73-B66E-039609481981}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="480" windowWidth="29040" windowHeight="15840" xr2:uid="{FB663B37-F28E-4922-8B1A-79EDB7B1DAD9}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
   <si>
     <t>FirstName</t>
   </si>
@@ -84,22 +84,16 @@
     <t>Jamol</t>
   </si>
   <si>
-    <t>C:\Users\Jama\Pictures\video_image-7jy607SNE.jpeg</t>
-  </si>
-  <si>
-    <t>C:\Users\Jama\Pictures\T02684PFZQE-U026MGFDQH2-115823339249-512.png</t>
-  </si>
-  <si>
-    <t>C:\Users\Jama\Pictures\scrum-team-2.png</t>
-  </si>
-  <si>
-    <t>anasule0012345</t>
-  </si>
-  <si>
-    <t>blakenailya0012345</t>
-  </si>
-  <si>
-    <t>mikeaj0012345</t>
+    <t>C:\Users\Jama\Pictures\testng-tutorial.png</t>
+  </si>
+  <si>
+    <t>anasule001234567</t>
+  </si>
+  <si>
+    <t>blakenailya001234567</t>
+  </si>
+  <si>
+    <t>mikeaj001234567</t>
   </si>
 </sst>
 </file>
@@ -465,7 +459,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -473,8 +467,8 @@
     <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14" customWidth="1"/>
+    <col min="5" max="5" width="19.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -512,7 +506,7 @@
         <v>16</v>
       </c>
       <c r="E2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>9</v>
@@ -529,10 +523,10 @@
         <v>12</v>
       </c>
       <c r="D3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>9</v>
@@ -549,10 +543,10 @@
         <v>15</v>
       </c>
       <c r="D4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>9</v>

</xml_diff>